<commit_message>
Novo Dataset ajustado pelo black, copia dos graficos para outra pasta (antigos).
</commit_message>
<xml_diff>
--- a/dados/COVID19IES.xlsx
+++ b/dados/COVID19IES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\with-a-little-help-from-my-friends\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpalbino/Library/Mobile Documents/com~apple~CloudDocs/GitHub/with-a-little-help-from-my-friends/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED27940-5362-4F60-817F-14E15426EB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CEFFD5-B541-DA43-8C7C-95D6715A81B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2352" yWindow="1452" windowWidth="18972" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2261" uniqueCount="396">
   <si>
     <t>Sim</t>
   </si>
@@ -900,12 +900,6 @@
     <t>É mais ou menos o mesmo</t>
   </si>
   <si>
-    <t>São mais ou menos os mesmos</t>
-  </si>
-  <si>
-    <t>São mais ou menos as mesmas</t>
-  </si>
-  <si>
     <t>Reconheço que minha instituição foi muito receptiva a dificuldade e dúvidas que os alunos tiveram ao longo do processo.</t>
   </si>
   <si>
@@ -918,9 +912,6 @@
     <t>Fundação Getúlio Vargas</t>
   </si>
   <si>
-    <t>Está mais ou menos o mesmo</t>
-  </si>
-  <si>
     <t>Não presenciei a alteração de dinâmica durante o curso (ingressei em 2021 na instituição), porém acredito que a produtividade aumentou. Atualmente tenho mais tempo focado na realização das tarefas que anteriormente.</t>
   </si>
   <si>
@@ -937,9 +928,6 @@
   </si>
   <si>
     <t>Reconhecendo o privilégio de poder trabalhar e estudar da minha casa, acredito que a pandemia impactou pouco meu cotidiano em questões econômicas ou de saúde. Uma observação possível é que a utilização do tempo melhorou. Mais atividades podem ser realizadas ao mesmo momento. Por outro lado, aspectos como distanciamento social e  incertezas sobre os meses futuros impactaram diretamente o psicológico.</t>
-  </si>
-  <si>
-    <t>Está/É mais ou menos o mesmo</t>
   </si>
   <si>
     <t>Alimentação, Outras (por favor, complemente):</t>
@@ -1228,7 +1216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1509,218 +1497,221 @@
   </sheetPr>
   <dimension ref="A1:BB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="AU19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="4.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="33.33203125" customWidth="1"/>
-    <col min="8" max="8" width="57.21875" customWidth="1"/>
+    <col min="8" max="8" width="57.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" style="3" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="11.5" customWidth="1"/>
+    <col min="14" max="14" width="14.5" customWidth="1"/>
     <col min="15" max="15" width="100.33203125" customWidth="1"/>
     <col min="16" max="16" width="14" style="3" customWidth="1"/>
-    <col min="17" max="17" width="60.88671875" customWidth="1"/>
-    <col min="18" max="20" width="18.88671875" customWidth="1"/>
-    <col min="21" max="21" width="16.77734375" customWidth="1"/>
-    <col min="22" max="22" width="102.109375" customWidth="1"/>
-    <col min="23" max="26" width="18.88671875" customWidth="1"/>
-    <col min="27" max="27" width="22.88671875" customWidth="1"/>
-    <col min="28" max="28" width="18.88671875" customWidth="1"/>
-    <col min="29" max="29" width="28.88671875" customWidth="1"/>
-    <col min="30" max="30" width="28.44140625" customWidth="1"/>
+    <col min="17" max="17" width="60.83203125" customWidth="1"/>
+    <col min="18" max="20" width="18.83203125" customWidth="1"/>
+    <col min="21" max="21" width="16.83203125" customWidth="1"/>
+    <col min="22" max="22" width="102.1640625" customWidth="1"/>
+    <col min="23" max="23" width="32.1640625" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" customWidth="1"/>
+    <col min="25" max="25" width="27.1640625" customWidth="1"/>
+    <col min="26" max="27" width="22.83203125" customWidth="1"/>
+    <col min="28" max="28" width="18.83203125" customWidth="1"/>
+    <col min="29" max="29" width="28.83203125" customWidth="1"/>
+    <col min="30" max="30" width="28.5" customWidth="1"/>
     <col min="31" max="31" width="26.6640625" customWidth="1"/>
-    <col min="32" max="32" width="25.88671875" customWidth="1"/>
+    <col min="32" max="32" width="25.83203125" customWidth="1"/>
     <col min="33" max="33" width="27.6640625" customWidth="1"/>
     <col min="34" max="34" width="25.33203125" customWidth="1"/>
-    <col min="35" max="35" width="52.21875" customWidth="1"/>
-    <col min="36" max="36" width="10.44140625" customWidth="1"/>
+    <col min="35" max="35" width="52.1640625" customWidth="1"/>
+    <col min="36" max="36" width="11" customWidth="1"/>
     <col min="37" max="37" width="66.6640625" customWidth="1"/>
-    <col min="38" max="38" width="28.5546875" customWidth="1"/>
-    <col min="39" max="39" width="30.77734375" customWidth="1"/>
-    <col min="40" max="40" width="25.88671875" customWidth="1"/>
+    <col min="38" max="38" width="28.5" customWidth="1"/>
+    <col min="39" max="39" width="30.83203125" customWidth="1"/>
+    <col min="40" max="40" width="25.83203125" customWidth="1"/>
     <col min="41" max="41" width="14" customWidth="1"/>
-    <col min="42" max="42" width="29.109375" customWidth="1"/>
-    <col min="43" max="43" width="84.44140625" customWidth="1"/>
-    <col min="44" max="44" width="23.109375" customWidth="1"/>
+    <col min="42" max="42" width="29.1640625" customWidth="1"/>
+    <col min="43" max="43" width="84.5" customWidth="1"/>
+    <col min="44" max="44" width="23.1640625" customWidth="1"/>
     <col min="45" max="45" width="26.6640625" customWidth="1"/>
-    <col min="46" max="49" width="18.88671875" customWidth="1"/>
-    <col min="50" max="50" width="21.44140625" customWidth="1"/>
-    <col min="51" max="51" width="21.21875" customWidth="1"/>
-    <col min="52" max="58" width="18.88671875" customWidth="1"/>
+    <col min="46" max="48" width="18.83203125" customWidth="1"/>
+    <col min="49" max="49" width="24.83203125" customWidth="1"/>
+    <col min="50" max="50" width="21.5" customWidth="1"/>
+    <col min="51" max="51" width="21.1640625" customWidth="1"/>
+    <col min="52" max="58" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="13">
       <c r="A1" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="AW1" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>367</v>
-      </c>
     </row>
-    <row r="2" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" ht="15.75" customHeight="1">
       <c r="A2" s="2">
         <v>44308.772397754627</v>
       </c>
@@ -1794,11 +1785,14 @@
         <v>12</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="AE2" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AF2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1808,8 +1802,11 @@
       <c r="AH2" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="AI2" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="AM2" s="1" t="s">
-        <v>292</v>
+        <v>62</v>
       </c>
       <c r="AN2" s="1" t="s">
         <v>25</v>
@@ -1818,7 +1815,7 @@
         <v>10</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="AQ2" s="1" t="s">
         <v>229</v>
@@ -1827,13 +1824,13 @@
         <v>28</v>
       </c>
       <c r="AT2" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="AV2" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="AW2" s="1" t="s">
         <v>37</v>
@@ -1845,7 +1842,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" ht="15.75" customHeight="1">
       <c r="A3" s="2">
         <v>44308.918698055553</v>
       </c>
@@ -1862,10 +1859,10 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>33</v>
@@ -1919,10 +1916,13 @@
         <v>12</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>80</v>
@@ -1931,10 +1931,13 @@
         <v>38</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="AM3" s="1" t="s">
         <v>24</v>
@@ -1952,34 +1955,34 @@
         <v>63</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="AS3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT3" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="AU3" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AW3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AX3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AY3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AZ3" s="1" t="s">
-        <v>304</v>
-      </c>
     </row>
-    <row r="4" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" ht="15.75" customHeight="1">
       <c r="A4" s="2">
         <v>44312.609396006941</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>156</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
@@ -2056,19 +2059,25 @@
         <v>12</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>305</v>
+        <v>16</v>
       </c>
       <c r="AD4" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="AE4" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AF4" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>291</v>
+        <v>20</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="AM4" s="1" t="s">
         <v>41</v>
@@ -2080,25 +2089,25 @@
         <v>10</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="AQ4" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="AS4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="AU4" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="AV4" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="AW4" s="1" t="s">
         <v>12</v>
@@ -2110,7 +2119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" ht="14">
       <c r="A5" s="2">
         <v>44337.639256956019</v>
       </c>
@@ -2130,7 +2139,7 @@
         <v>156</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>5</v>
@@ -2187,19 +2196,25 @@
         <v>37</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>305</v>
+        <v>16</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="AE5" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AF5" s="1" t="s">
-        <v>291</v>
+        <v>19</v>
       </c>
       <c r="AG5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="AM5" s="1" t="s">
         <v>24</v>
@@ -2211,7 +2226,7 @@
         <v>10</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="AQ5" s="1" t="s">
         <v>27</v>
@@ -2220,13 +2235,13 @@
         <v>28</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="AW5" s="1" t="s">
         <v>37</v>
@@ -2238,7 +2253,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" ht="13">
       <c r="A6" s="2">
         <v>44490.349946111106</v>
       </c>
@@ -2261,7 +2276,7 @@
         <v>156</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>77</v>
@@ -2312,34 +2327,34 @@
         <v>37</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>305</v>
+        <v>16</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>291</v>
+        <v>19</v>
       </c>
       <c r="AG6" s="1" t="s">
         <v>291</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
       </c>
       <c r="AI6" s="1" t="s">
         <v>245</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AM6" s="1" t="s">
-        <v>292</v>
+        <v>62</v>
       </c>
       <c r="AN6" s="1" t="s">
         <v>42</v>
@@ -2348,16 +2363,16 @@
         <v>10</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="AS6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AU6" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="AW6" s="1" t="s">
         <v>15</v>
@@ -2369,7 +2384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" ht="13">
       <c r="A7" s="2">
         <v>44645.433733912039</v>
       </c>
@@ -2392,7 +2407,7 @@
         <v>156</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>5</v>
@@ -2497,7 +2512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" ht="15.75" customHeight="1">
       <c r="A8" s="2">
         <v>44645.571748668983</v>
       </c>
@@ -2631,7 +2646,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>44645.603025405093</v>
       </c>
@@ -2774,7 +2789,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" ht="15.75" customHeight="1">
       <c r="A10" s="2">
         <v>44645.610024664347</v>
       </c>
@@ -2797,7 +2812,7 @@
         <v>156</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>33</v>
@@ -2929,7 +2944,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" ht="15.75" customHeight="1">
       <c r="A11" s="2">
         <v>44645.984089571764</v>
       </c>
@@ -2952,7 +2967,7 @@
         <v>156</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>193</v>
@@ -3084,7 +3099,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" ht="15.75" customHeight="1">
       <c r="A12" s="2">
         <v>44646.398636967591</v>
       </c>
@@ -3239,7 +3254,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" ht="15.75" customHeight="1">
       <c r="A13" s="2">
         <v>44646.484321793978</v>
       </c>
@@ -3262,7 +3277,7 @@
         <v>156</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>33</v>
@@ -3379,7 +3394,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" ht="15.75" customHeight="1">
       <c r="A14" s="2">
         <v>44646.512648807868</v>
       </c>
@@ -3534,7 +3549,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" ht="15.75" customHeight="1">
       <c r="A15" s="2">
         <v>44647.485230532402</v>
       </c>
@@ -3668,7 +3683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" ht="15.75" customHeight="1">
       <c r="A16" s="2">
         <v>44647.676722037038</v>
       </c>
@@ -3805,7 +3820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" ht="15.75" customHeight="1">
       <c r="A17" s="2">
         <v>44647.921008333331</v>
       </c>
@@ -3828,7 +3843,7 @@
         <v>156</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>5</v>
@@ -3936,7 +3951,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" ht="15.75" customHeight="1">
       <c r="A18" s="2">
         <v>44647.976546481485</v>
       </c>
@@ -4064,7 +4079,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" ht="15.75" customHeight="1">
       <c r="A19" s="2">
         <v>44648.717444837966</v>
       </c>
@@ -4087,7 +4102,7 @@
         <v>156</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>33</v>
@@ -4210,7 +4225,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" ht="15.75" customHeight="1">
       <c r="A20" s="2">
         <v>44649.769038090279</v>
       </c>
@@ -4233,7 +4248,7 @@
         <v>156</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>33</v>
@@ -4356,7 +4371,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" ht="15.75" customHeight="1">
       <c r="A21" s="2">
         <v>44651.400174710652</v>
       </c>
@@ -4514,7 +4529,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="22" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" ht="15.75" customHeight="1">
       <c r="A22" s="2">
         <v>44669.433834733798</v>
       </c>
@@ -4657,7 +4672,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" ht="15.75" customHeight="1">
       <c r="A23" s="2">
         <v>44669.463378217595</v>
       </c>
@@ -4785,7 +4800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" ht="15.75" customHeight="1">
       <c r="A24" s="2">
         <v>44669.522761319444</v>
       </c>
@@ -4916,7 +4931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" ht="15.75" customHeight="1">
       <c r="A25" s="2">
         <v>44669.675171030089</v>
       </c>
@@ -5047,7 +5062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" ht="15.75" customHeight="1">
       <c r="A26" s="2">
         <v>44669.966824780087</v>
       </c>
@@ -5178,7 +5193,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" ht="15.75" customHeight="1">
       <c r="A27" s="2">
         <v>44669.968822025461</v>
       </c>
@@ -5318,7 +5333,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" ht="15.75" customHeight="1">
       <c r="A28" s="2">
         <v>44670.671746284723</v>
       </c>
@@ -5406,6 +5421,9 @@
       <c r="AE28" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="AF28" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AG28" s="1" t="s">
         <v>25</v>
       </c>
@@ -5458,7 +5476,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" ht="15.75" customHeight="1">
       <c r="A29" s="2">
         <v>44670.771344768524</v>
       </c>
@@ -5598,7 +5616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" ht="15.75" customHeight="1">
       <c r="A30" s="2">
         <v>44754.453575532403</v>
       </c>
@@ -5738,7 +5756,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" ht="15.75" customHeight="1">
       <c r="A31" s="2">
         <v>44879.894109953704</v>
       </c>
@@ -5761,7 +5779,7 @@
         <v>156</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>5</v>
@@ -5872,7 +5890,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:52" ht="15.75" customHeight="1">
       <c r="A32" s="2">
         <v>44880.347730717593</v>
       </c>
@@ -5895,7 +5913,7 @@
         <v>156</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>33</v>
@@ -6000,7 +6018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:52" ht="15.75" customHeight="1">
       <c r="A33" s="2">
         <v>44881.627196759262</v>
       </c>
@@ -6023,7 +6041,7 @@
         <v>156</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>33</v>
@@ -6149,7 +6167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:52" ht="15.75" customHeight="1">
       <c r="A34" s="2">
         <v>44883.582158321762</v>
       </c>
@@ -6172,7 +6190,7 @@
         <v>156</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>5</v>
@@ -6289,7 +6307,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:52" ht="15.75" customHeight="1">
       <c r="A35" s="2">
         <v>44885.785295578702</v>
       </c>
@@ -6312,7 +6330,7 @@
         <v>156</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>5</v>
@@ -6435,7 +6453,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:52" ht="15.75" customHeight="1">
       <c r="A36" s="2">
         <v>44885.839950104171</v>
       </c>
@@ -6581,7 +6599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:52" ht="15.75" customHeight="1">
       <c r="A37" s="2">
         <v>44885.841205833334</v>
       </c>
@@ -6712,7 +6730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:52" ht="15.75" customHeight="1">
       <c r="A38" s="2">
         <v>44886.642705254635</v>
       </c>
@@ -6735,7 +6753,7 @@
         <v>156</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>5</v>
@@ -6867,7 +6885,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:52" ht="15.75" customHeight="1">
       <c r="A39" s="2">
         <v>44886.644437581017</v>
       </c>
@@ -6890,7 +6908,7 @@
         <v>101</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>33</v>
@@ -7010,7 +7028,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:52" ht="15.75" customHeight="1">
       <c r="A40" s="2">
         <v>44886.649916111113</v>
       </c>
@@ -7033,7 +7051,7 @@
         <v>156</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>33</v>
@@ -7138,7 +7156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:52" ht="15.75" customHeight="1">
       <c r="A41" s="2">
         <v>44886.684875196763</v>
       </c>
@@ -7161,7 +7179,7 @@
         <v>101</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>33</v>
@@ -7287,7 +7305,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:52" ht="15.75" customHeight="1">
       <c r="A42" s="2">
         <v>44886.748539513894</v>
       </c>
@@ -7424,7 +7442,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:52" ht="15.75" customHeight="1">
       <c r="A43" s="2">
         <v>44886.767306041671</v>
       </c>
@@ -7564,7 +7582,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:52" ht="15.75" customHeight="1">
       <c r="A44" s="2">
         <v>44886.878623761571</v>
       </c>
@@ -7692,7 +7710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:52" ht="15.75" customHeight="1">
       <c r="A45" s="2">
         <v>44886.924897337958</v>
       </c>
@@ -7820,7 +7838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:52" ht="15.75" customHeight="1">
       <c r="A46" s="2">
         <v>44886.958313206022</v>
       </c>
@@ -7843,7 +7861,7 @@
         <v>156</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>33</v>
@@ -7957,7 +7975,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:52" ht="15.75" customHeight="1">
       <c r="A47" s="2">
         <v>44888.341911099538</v>
       </c>
@@ -7977,7 +7995,7 @@
         <v>32</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>138</v>
@@ -8112,7 +8130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:52" ht="15.75" customHeight="1">
       <c r="A48" s="2">
         <v>44895.541855706018</v>
       </c>
@@ -8135,7 +8153,7 @@
         <v>156</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>5</v>
@@ -8264,7 +8282,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:54" ht="15.75" customHeight="1">
       <c r="A49" s="2">
         <v>44899.894309016207</v>
       </c>
@@ -8287,7 +8305,7 @@
         <v>156</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>5</v>
@@ -8407,7 +8425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:54" ht="15.75" customHeight="1">
       <c r="A50" s="2">
         <v>44900.956294351854</v>
       </c>
@@ -8430,7 +8448,7 @@
         <v>156</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>5</v>
@@ -8556,7 +8574,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:54" ht="15.75" customHeight="1">
       <c r="A51" s="2">
         <v>44901.570091388887</v>
       </c>
@@ -8579,7 +8597,7 @@
         <v>156</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>5</v>
@@ -8696,7 +8714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:54" ht="15.75" customHeight="1">
       <c r="A52" s="7">
         <v>44907</v>
       </c>
@@ -8710,19 +8728,19 @@
         <v>44</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="J52" s="6">
         <v>44046</v>
@@ -8740,7 +8758,7 @@
         <v>10</v>
       </c>
       <c r="O52" s="8" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="P52" s="4"/>
       <c r="Q52" s="4" t="s">
@@ -8777,7 +8795,7 @@
         <v>30</v>
       </c>
       <c r="AB52" s="4" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="AC52" s="4" t="s">
         <v>48</v>
@@ -8805,7 +8823,7 @@
         <v>23</v>
       </c>
       <c r="AL52" s="4" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="AM52" s="4" t="s">
         <v>62</v>
@@ -8820,22 +8838,22 @@
         <v>26</v>
       </c>
       <c r="AQ52" s="4" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AR52" s="4" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AS52" s="4" t="s">
         <v>82</v>
       </c>
       <c r="AT52" s="4" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AU52" s="4" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="AV52" s="4" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AW52" s="4" t="s">
         <v>91</v>
@@ -8847,12 +8865,12 @@
         <v>91</v>
       </c>
       <c r="AZ52" s="4" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="BA52" s="4"/>
       <c r="BB52" s="4"/>
     </row>
-    <row r="53" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:54" ht="15.75" customHeight="1">
       <c r="A53" s="7">
         <v>44908</v>
       </c>
@@ -8875,7 +8893,7 @@
         <v>156</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>33</v>
@@ -8933,7 +8951,7 @@
         <v>15</v>
       </c>
       <c r="AB53" s="4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="AC53" s="4" t="s">
         <v>16</v>
@@ -8961,7 +8979,7 @@
         <v>23</v>
       </c>
       <c r="AL53" s="4" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="AM53" s="4" t="s">
         <v>24</v>
@@ -8976,22 +8994,22 @@
         <v>26</v>
       </c>
       <c r="AQ53" s="4" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="AR53" s="4" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="AS53" s="4" t="s">
         <v>53</v>
       </c>
       <c r="AT53" s="4" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="AU53" s="4" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="AV53" s="4" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="AW53" s="4" t="s">
         <v>15</v>

</xml_diff>